<commit_message>
Quinto Commit: Execução Final
</commit_message>
<xml_diff>
--- a/data/gold/gold_sla_by_analyst.xlsx
+++ b/data/gold/gold_sla_by_analyst.xlsx
@@ -448,7 +448,7 @@
         <v>148</v>
       </c>
       <c r="C2" t="n">
-        <v>53.51351351351352</v>
+        <v>37.61313626083334</v>
       </c>
     </row>
     <row r="3">
@@ -461,7 +461,7 @@
         <v>175</v>
       </c>
       <c r="C3" t="n">
-        <v>54.03428571428572</v>
+        <v>38.43518730115238</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         <v>175</v>
       </c>
       <c r="C4" t="n">
-        <v>56.50285714285715</v>
+        <v>39.66689682492857</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +487,7 @@
         <v>157</v>
       </c>
       <c r="C5" t="n">
-        <v>53.19745222929937</v>
+        <v>38.41266454308918</v>
       </c>
     </row>
     <row r="6">
@@ -500,7 +500,7 @@
         <v>149</v>
       </c>
       <c r="C6" t="n">
-        <v>49.77181208053691</v>
+        <v>34.99892058125839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>